<commit_message>
Added photos for each of the incumbents.
</commit_message>
<xml_diff>
--- a/assets/background/data_collection/Senator_Data_21116.xlsx
+++ b/assets/background/data_collection/Senator_Data_21116.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brmayes/Desktop/*Spring 2016/583/Projects/senator-dataApp/background/data_collection/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brmayes/Desktop/*Spring 2016/583/Projects/senator-dataApp/assets/background/data_collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6740" yWindow="460" windowWidth="22060" windowHeight="13260" tabRatio="500"/>
+    <workbookView xWindow="10640" yWindow="460" windowWidth="18160" windowHeight="15940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="All Senators" sheetId="3" r:id="rId1"/>
@@ -1109,7 +1109,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1187,6 +1187,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1235,7 +1241,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1288,6 +1294,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1585,8 +1594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="97" zoomScaleNormal="97" zoomScalePageLayoutView="97" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" zoomScalePageLayoutView="97" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1648,7 +1657,7 @@
         <v>2021</v>
       </c>
       <c r="G2" s="5" t="b">
-        <f>IF(F2 = 2017,TRUE,FALSE)</f>
+        <f t="shared" ref="G2:G33" si="0">IF(F2 = 2017,TRUE,FALSE)</f>
         <v>0</v>
       </c>
     </row>
@@ -1672,7 +1681,7 @@
         <v>2021</v>
       </c>
       <c r="G3" s="5" t="b">
-        <f>IF(F3 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1696,7 +1705,7 @@
         <v>2019</v>
       </c>
       <c r="G4" s="5" t="b">
-        <f>IF(F4 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1720,7 +1729,7 @@
         <v>2021</v>
       </c>
       <c r="G5" s="5" t="b">
-        <f>IF(F5 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1744,7 +1753,7 @@
         <v>2019</v>
       </c>
       <c r="G6" s="5" t="b">
-        <f>IF(F6 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1768,7 +1777,7 @@
         <v>2021</v>
       </c>
       <c r="G7" s="5" t="b">
-        <f>IF(F7 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1792,7 +1801,7 @@
         <v>2019</v>
       </c>
       <c r="G8" s="5" t="b">
-        <f>IF(F8 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1816,7 +1825,7 @@
         <v>2021</v>
       </c>
       <c r="G9" s="5" t="b">
-        <f>IF(F9 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1840,7 +1849,7 @@
         <v>2019</v>
       </c>
       <c r="G10" s="5" t="b">
-        <f>IF(F10 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1864,7 +1873,7 @@
         <v>2019</v>
       </c>
       <c r="G11" s="5" t="b">
-        <f>IF(F11 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1888,7 +1897,7 @@
         <v>2021</v>
       </c>
       <c r="G12" s="5" t="b">
-        <f>IF(F12 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1912,7 +1921,7 @@
         <v>2019</v>
       </c>
       <c r="G13" s="5" t="b">
-        <f>IF(F13 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1936,7 +1945,7 @@
         <v>2021</v>
       </c>
       <c r="G14" s="5" t="b">
-        <f>IF(F14 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1960,7 +1969,7 @@
         <v>2021</v>
       </c>
       <c r="G15" s="5" t="b">
-        <f>IF(F15 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1984,7 +1993,7 @@
         <v>2019</v>
       </c>
       <c r="G16" s="5" t="b">
-        <f>IF(F16 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2008,7 +2017,7 @@
         <v>2021</v>
       </c>
       <c r="G17" s="5" t="b">
-        <f>IF(F17 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2032,7 +2041,7 @@
         <v>2021</v>
       </c>
       <c r="G18" s="5" t="b">
-        <f>IF(F18 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2056,7 +2065,7 @@
         <v>2021</v>
       </c>
       <c r="G19" s="5" t="b">
-        <f>IF(F19 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2080,7 +2089,7 @@
         <v>2021</v>
       </c>
       <c r="G20" s="5" t="b">
-        <f>IF(F20 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2104,7 +2113,7 @@
         <v>2019</v>
       </c>
       <c r="G21" s="5" t="b">
-        <f>IF(F21 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2128,7 +2137,7 @@
         <v>2021</v>
       </c>
       <c r="G22" s="5" t="b">
-        <f>IF(F22 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2152,7 +2161,7 @@
         <v>2019</v>
       </c>
       <c r="G23" s="5" t="b">
-        <f>IF(F23 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2176,7 +2185,7 @@
         <v>2021</v>
       </c>
       <c r="G24" s="5" t="b">
-        <f>IF(F24 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2200,7 +2209,7 @@
         <v>2019</v>
       </c>
       <c r="G25" s="5" t="b">
-        <f>IF(F25 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2224,7 +2233,7 @@
         <v>2021</v>
       </c>
       <c r="G26" s="5" t="b">
-        <f>IF(F26 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2248,7 +2257,7 @@
         <v>2019</v>
       </c>
       <c r="G27" s="5" t="b">
-        <f>IF(F27 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2272,7 +2281,7 @@
         <v>2021</v>
       </c>
       <c r="G28" s="5" t="b">
-        <f>IF(F28 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2296,7 +2305,7 @@
         <v>2019</v>
       </c>
       <c r="G29" s="5" t="b">
-        <f>IF(F29 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2320,7 +2329,7 @@
         <v>2021</v>
       </c>
       <c r="G30" s="5" t="b">
-        <f>IF(F30 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2344,7 +2353,7 @@
         <v>2019</v>
       </c>
       <c r="G31" s="5" t="b">
-        <f>IF(F31 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2368,7 +2377,7 @@
         <v>2019</v>
       </c>
       <c r="G32" s="5" t="b">
-        <f>IF(F32 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2392,7 +2401,7 @@
         <v>2019</v>
       </c>
       <c r="G33" s="5" t="b">
-        <f>IF(F33 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I33" s="20"/>
@@ -2417,7 +2426,7 @@
         <v>2021</v>
       </c>
       <c r="G34" s="5" t="b">
-        <f>IF(F34 = 2017,TRUE,FALSE)</f>
+        <f t="shared" ref="G34:G65" si="1">IF(F34 = 2017,TRUE,FALSE)</f>
         <v>0</v>
       </c>
       <c r="I34" s="20"/>
@@ -2442,7 +2451,7 @@
         <v>2021</v>
       </c>
       <c r="G35" s="5" t="b">
-        <f>IF(F35 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I35" s="20"/>
@@ -2467,7 +2476,7 @@
         <v>2019</v>
       </c>
       <c r="G36" s="5" t="b">
-        <f>IF(F36 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I36" s="20"/>
@@ -2492,7 +2501,7 @@
         <v>2019</v>
       </c>
       <c r="G37" s="5" t="b">
-        <f>IF(F37 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I37" s="20"/>
@@ -2517,7 +2526,7 @@
         <v>2021</v>
       </c>
       <c r="G38" s="5" t="b">
-        <f>IF(F38 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I38" s="20"/>
@@ -2542,7 +2551,7 @@
         <v>2021</v>
       </c>
       <c r="G39" s="5" t="b">
-        <f>IF(F39 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I39" s="20"/>
@@ -2567,7 +2576,7 @@
         <v>2019</v>
       </c>
       <c r="G40" s="5" t="b">
-        <f>IF(F40 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I40" s="20"/>
@@ -2592,7 +2601,7 @@
         <v>2021</v>
       </c>
       <c r="G41" s="5" t="b">
-        <f>IF(F41 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I41" s="20"/>
@@ -2617,7 +2626,7 @@
         <v>2019</v>
       </c>
       <c r="G42" s="5" t="b">
-        <f>IF(F42 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I42" s="20"/>
@@ -2642,7 +2651,7 @@
         <v>2019</v>
       </c>
       <c r="G43" s="5" t="b">
-        <f>IF(F43 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I43" s="20"/>
@@ -2667,7 +2676,7 @@
         <v>2021</v>
       </c>
       <c r="G44" s="5" t="b">
-        <f>IF(F44 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I44" s="20"/>
@@ -2692,7 +2701,7 @@
         <v>2019</v>
       </c>
       <c r="G45" s="5" t="b">
-        <f>IF(F45 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I45" s="20"/>
@@ -2717,7 +2726,7 @@
         <v>2019</v>
       </c>
       <c r="G46" s="5" t="b">
-        <f>IF(F46 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I46" s="20"/>
@@ -2742,7 +2751,7 @@
         <v>2021</v>
       </c>
       <c r="G47" s="5" t="b">
-        <f>IF(F47 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I47" s="20"/>
@@ -2767,7 +2776,7 @@
         <v>2021</v>
       </c>
       <c r="G48" s="5" t="b">
-        <f>IF(F48 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I48" s="20"/>
@@ -2792,7 +2801,7 @@
         <v>2019</v>
       </c>
       <c r="G49" s="5" t="b">
-        <f>IF(F49 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I49" s="20"/>
@@ -2817,7 +2826,7 @@
         <v>2021</v>
       </c>
       <c r="G50" s="5" t="b">
-        <f>IF(F50 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I50" s="20"/>
@@ -2842,7 +2851,7 @@
         <v>2019</v>
       </c>
       <c r="G51" s="5" t="b">
-        <f>IF(F51 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I51" s="20"/>
@@ -2867,7 +2876,7 @@
         <v>2021</v>
       </c>
       <c r="G52" s="5" t="b">
-        <f>IF(F52 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I52" s="20"/>
@@ -2892,7 +2901,7 @@
         <v>2021</v>
       </c>
       <c r="G53" s="5" t="b">
-        <f>IF(F53 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I53" s="20"/>
@@ -2917,7 +2926,7 @@
         <v>2021</v>
       </c>
       <c r="G54" s="5" t="b">
-        <f>IF(F54 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I54" s="20"/>
@@ -2942,7 +2951,7 @@
         <v>2019</v>
       </c>
       <c r="G55" s="5" t="b">
-        <f>IF(F55 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I55" s="20"/>
@@ -2967,7 +2976,7 @@
         <v>2021</v>
       </c>
       <c r="G56" s="5" t="b">
-        <f>IF(F56 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I56" s="20"/>
@@ -2992,7 +3001,7 @@
         <v>2019</v>
       </c>
       <c r="G57" s="5" t="b">
-        <f>IF(F57 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I57" s="20"/>
@@ -3017,7 +3026,7 @@
         <v>2019</v>
       </c>
       <c r="G58" s="5" t="b">
-        <f>IF(F58 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I58" s="20"/>
@@ -3042,7 +3051,7 @@
         <v>2019</v>
       </c>
       <c r="G59" s="5" t="b">
-        <f>IF(F59 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I59" s="20"/>
@@ -3067,7 +3076,7 @@
         <v>2021</v>
       </c>
       <c r="G60" s="5" t="b">
-        <f>IF(F60 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I60" s="20"/>
@@ -3092,7 +3101,7 @@
         <v>2019</v>
       </c>
       <c r="G61" s="5" t="b">
-        <f>IF(F61 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I61" s="20"/>
@@ -3117,7 +3126,7 @@
         <v>2019</v>
       </c>
       <c r="G62" s="5" t="b">
-        <f>IF(F62 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I62" s="20"/>
@@ -3142,7 +3151,7 @@
         <v>2019</v>
       </c>
       <c r="G63" s="5" t="b">
-        <f>IF(F63 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I63" s="20"/>
@@ -3167,7 +3176,7 @@
         <v>2021</v>
       </c>
       <c r="G64" s="5" t="b">
-        <f>IF(F64 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I64" s="20"/>
@@ -3192,7 +3201,7 @@
         <v>2019</v>
       </c>
       <c r="G65" s="5" t="b">
-        <f>IF(F65 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I65" s="20"/>
@@ -3217,7 +3226,7 @@
         <v>2021</v>
       </c>
       <c r="G66" s="5" t="b">
-        <f>IF(F66 = 2017,TRUE,FALSE)</f>
+        <f t="shared" ref="G66:G97" si="2">IF(F66 = 2017,TRUE,FALSE)</f>
         <v>0</v>
       </c>
       <c r="I66" s="20"/>
@@ -3242,13 +3251,13 @@
         <v>2019</v>
       </c>
       <c r="G67" s="5" t="b">
-        <f>IF(F67 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I67" s="20"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
+      <c r="A68" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B68" s="24">
@@ -3267,7 +3276,7 @@
         <v>2017</v>
       </c>
       <c r="G68" s="5" t="b">
-        <f>IF(F68 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I68" s="20"/>
@@ -3292,7 +3301,7 @@
         <v>2017</v>
       </c>
       <c r="G69" s="5" t="b">
-        <f>IF(F69 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I69" s="20"/>
@@ -3317,7 +3326,7 @@
         <v>2017</v>
       </c>
       <c r="G70" s="5" t="b">
-        <f>IF(F70 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I70" s="20"/>
@@ -3342,7 +3351,7 @@
         <v>2017</v>
       </c>
       <c r="G71" s="5" t="b">
-        <f>IF(F71 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I71" s="20"/>
@@ -3367,7 +3376,7 @@
         <v>2017</v>
       </c>
       <c r="G72" s="5" t="b">
-        <f>IF(F72 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H72" s="5" t="s">
@@ -3395,7 +3404,7 @@
         <v>2017</v>
       </c>
       <c r="G73" s="5" t="b">
-        <f>IF(F73 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I73" s="20"/>
@@ -3420,7 +3429,7 @@
         <v>2017</v>
       </c>
       <c r="G74" s="5" t="b">
-        <f>IF(F74 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I74" s="20"/>
@@ -3445,7 +3454,7 @@
         <v>2017</v>
       </c>
       <c r="G75" s="5" t="b">
-        <f>IF(F75 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H75" s="5" t="s">
@@ -3473,7 +3482,7 @@
         <v>2017</v>
       </c>
       <c r="G76" s="5" t="b">
-        <f>IF(F76 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I76" s="20"/>
@@ -3498,7 +3507,7 @@
         <v>2017</v>
       </c>
       <c r="G77" s="5" t="b">
-        <f>IF(F77 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I77" s="20"/>
@@ -3523,7 +3532,7 @@
         <v>2017</v>
       </c>
       <c r="G78" s="5" t="b">
-        <f>IF(F78 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I78" s="20"/>
@@ -3548,7 +3557,7 @@
         <v>2017</v>
       </c>
       <c r="G79" s="5" t="b">
-        <f>IF(F79 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I79" s="20"/>
@@ -3573,7 +3582,7 @@
         <v>2017</v>
       </c>
       <c r="G80" s="5" t="b">
-        <f>IF(F80 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H80" s="5" t="s">
@@ -3601,7 +3610,7 @@
         <v>2017</v>
       </c>
       <c r="G81" s="5" t="b">
-        <f>IF(F81 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I81" s="20"/>
@@ -3626,7 +3635,7 @@
         <v>2017</v>
       </c>
       <c r="G82" s="5" t="b">
-        <f>IF(F82 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I82" s="20"/>
@@ -3651,7 +3660,7 @@
         <v>2017</v>
       </c>
       <c r="G83" s="5" t="b">
-        <f>IF(F83 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3675,7 +3684,7 @@
         <v>2017</v>
       </c>
       <c r="G84" s="5" t="b">
-        <f>IF(F84 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H84" s="5" t="s">
@@ -3702,7 +3711,7 @@
         <v>2017</v>
       </c>
       <c r="G85" s="5" t="b">
-        <f>IF(F85 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H85" s="5" t="s">
@@ -3729,7 +3738,7 @@
         <v>2017</v>
       </c>
       <c r="G86" s="5" t="b">
-        <f>IF(F86 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3753,7 +3762,7 @@
         <v>2017</v>
       </c>
       <c r="G87" s="5" t="b">
-        <f>IF(F87 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H87" s="5" t="s">
@@ -3780,7 +3789,7 @@
         <v>2017</v>
       </c>
       <c r="G88" s="5" t="b">
-        <f>IF(F88 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3804,7 +3813,7 @@
         <v>2017</v>
       </c>
       <c r="G89" s="5" t="b">
-        <f>IF(F89 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3828,7 +3837,7 @@
         <v>2017</v>
       </c>
       <c r="G90" s="5" t="b">
-        <f>IF(F90 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3852,7 +3861,7 @@
         <v>2017</v>
       </c>
       <c r="G91" s="5" t="b">
-        <f>IF(F91 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3876,7 +3885,7 @@
         <v>2017</v>
       </c>
       <c r="G92" s="5" t="b">
-        <f>IF(F92 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3900,7 +3909,7 @@
         <v>2017</v>
       </c>
       <c r="G93" s="5" t="b">
-        <f>IF(F93 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H93" s="5" t="s">
@@ -3927,7 +3936,7 @@
         <v>2017</v>
       </c>
       <c r="G94" s="5" t="b">
-        <f>IF(F94 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3951,7 +3960,7 @@
         <v>2017</v>
       </c>
       <c r="G95" s="5" t="b">
-        <f>IF(F95 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3975,7 +3984,7 @@
         <v>2017</v>
       </c>
       <c r="G96" s="5" t="b">
-        <f>IF(F96 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -3999,7 +4008,7 @@
         <v>2017</v>
       </c>
       <c r="G97" s="5" t="b">
-        <f>IF(F97 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -4023,7 +4032,7 @@
         <v>2017</v>
       </c>
       <c r="G98" s="5" t="b">
-        <f>IF(F98 = 2017,TRUE,FALSE)</f>
+        <f t="shared" ref="G98:G129" si="3">IF(F98 = 2017,TRUE,FALSE)</f>
         <v>1</v>
       </c>
     </row>
@@ -4047,7 +4056,7 @@
         <v>2017</v>
       </c>
       <c r="G99" s="5" t="b">
-        <f>IF(F99 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -4071,7 +4080,7 @@
         <v>2017</v>
       </c>
       <c r="G100" s="5" t="b">
-        <f>IF(F100 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -4095,7 +4104,7 @@
         <v>2017</v>
       </c>
       <c r="G101" s="5" t="b">
-        <f>IF(F101 = 2017,TRUE,FALSE)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>